<commit_message>
fixinig import and goods worker amd purchuses
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flutter_saffoury_paper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F8FF45-8ACD-41C4-9A16-6486AADE2D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>Customs Clearances</t>
   </si>
@@ -76,9 +82,6 @@
     <t>2020-01-23 12:56:47</t>
   </si>
   <si>
-    <t>2822426428002</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -94,28 +97,22 @@
     <t>2020-01-24 12:56:47</t>
   </si>
   <si>
-    <t>2765243718001</t>
-  </si>
-  <si>
     <t>2020-01-21 12:56:47</t>
   </si>
   <si>
-    <t>2765243718002</t>
-  </si>
-  <si>
-    <t>2765243718003</t>
-  </si>
-  <si>
     <t>Size:Width</t>
   </si>
   <si>
     <t>Size:Length</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -150,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -163,6 +160,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -365,19 +365,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="43.3046875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="37.299999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,13 +418,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -452,11 +458,11 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2">
+        <v>1000</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
       </c>
       <c r="M2">
         <v>540</v>
@@ -464,8 +470,11 @@
       <c r="N2">
         <v>0</v>
       </c>
+      <c r="O2">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -473,13 +482,13 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -491,16 +500,16 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
-        <v>26</v>
+      <c r="K3">
+        <v>1001</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>520</v>
@@ -508,8 +517,11 @@
       <c r="N3">
         <v>600</v>
       </c>
+      <c r="O3">
+        <v>1001</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -517,13 +529,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -535,16 +547,16 @@
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
-        <v>28</v>
+      <c r="K4">
+        <v>1002</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>520</v>
@@ -552,8 +564,11 @@
       <c r="N4">
         <v>600</v>
       </c>
+      <c r="O4">
+        <v>1002</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -561,13 +576,13 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -579,22 +594,25 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="K5" t="s">
-        <v>29</v>
+      <c r="K5">
+        <v>1003</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>520</v>
       </c>
       <c r="N5">
         <v>600</v>
+      </c>
+      <c r="O5">
+        <v>1003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>